<commit_message>
dimensions checking, converstion to text
git-svn-id: https://svn.ecdf.ed.ac.uk/repo/biology/biodare@2416 b325261a-90cb-4c4b-9a13-2f556971fe3a
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/synthsys/util/excel/2CSVTest.xlsx
+++ b/src/test/resources/ed/synthsys/util/excel/2CSVTest.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>A</t>
   </si>
@@ -26,6 +27,9 @@
   </si>
   <si>
     <t>with,comma</t>
+  </si>
+  <si>
+    <t>I am not second sheet not to be readed</t>
   </si>
 </sst>
 </file>
@@ -380,7 +384,7 @@
   <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,4 +437,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>